<commit_message>
face rec before morphing and excel with results
</commit_message>
<xml_diff>
--- a/data/before_recognition.xlsx
+++ b/data/before_recognition.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murie\Documents\school\master\1B\Introduction2Biometrics\project_git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59FF15F8-D6F9-45A7-9B9B-DBE496581A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D9A8AD-F2DF-45CF-BF5B-891E7D240B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD5D7408-1DBF-4EC5-8EFD-A3374FDE4ED6}"/>
+    <workbookView xWindow="-7368" yWindow="3516" windowWidth="17280" windowHeight="8964" xr2:uid="{CD5D7408-1DBF-4EC5-8EFD-A3374FDE4ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,177 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>0.25822784827393636</t>
+    <t>wrong</t>
   </si>
   <si>
-    <t>0.11612819053479236</t>
-  </si>
-  <si>
-    <t>0.13036533017950483</t>
-  </si>
-  <si>
-    <t>0.2893757417230654</t>
-  </si>
-  <si>
-    <t>0.13633115512315744</t>
-  </si>
-  <si>
-    <t>0.2479468030317612</t>
-  </si>
-  <si>
-    <t>0.20879652971548748</t>
-  </si>
-  <si>
-    <t>0.3477561630742474</t>
-  </si>
-  <si>
-    <t>0.2809078920446832</t>
-  </si>
-  <si>
-    <t>0.17969332403533672</t>
-  </si>
-  <si>
-    <t>0.1803984103639685</t>
-  </si>
-  <si>
-    <t>0.2243254793445718</t>
-  </si>
-  <si>
-    <t>0.2754426680560811</t>
-  </si>
-  <si>
-    <t>0.32596346610592597</t>
-  </si>
-  <si>
-    <t>0.13101780533404442</t>
-  </si>
-  <si>
-    <t>0.1996135152835896</t>
-  </si>
-  <si>
-    <t>0.22473430028538632</t>
-  </si>
-  <si>
-    <t>0.24720502825847052</t>
-  </si>
-  <si>
-    <t>0.18242351820062447</t>
-  </si>
-  <si>
-    <t>0.09065309962439479</t>
-  </si>
-  <si>
-    <t>0.3093933234386399</t>
-  </si>
-  <si>
-    <t>0.19137676436157622</t>
-  </si>
-  <si>
-    <t>0.18197628385270861</t>
-  </si>
-  <si>
-    <t>0.11722804997760841</t>
-  </si>
-  <si>
-    <t>0.2559541613167712</t>
-  </si>
-  <si>
-    <t>0.15489158293399383</t>
-  </si>
-  <si>
-    <t>0.07882219200083496</t>
-  </si>
-  <si>
-    <t>0.2203245433974791</t>
-  </si>
-  <si>
-    <t>0.23479460176716208</t>
-  </si>
-  <si>
-    <t>0.18117627791668361</t>
-  </si>
-  <si>
-    <t>0.2881338621679199</t>
-  </si>
-  <si>
-    <t>0.2986819155228605</t>
-  </si>
-  <si>
-    <t>0.14550500436669084</t>
-  </si>
-  <si>
-    <t>0.3495402144003355</t>
-  </si>
-  <si>
-    <t>0.11702270756949869</t>
-  </si>
-  <si>
-    <t>0.2030426810242196</t>
-  </si>
-  <si>
-    <t>0.20735860639820156</t>
-  </si>
-  <si>
-    <t>0.24269776523380718</t>
-  </si>
-  <si>
-    <t>0.1300548914693919</t>
-  </si>
-  <si>
-    <t>0.29211588888628537</t>
-  </si>
-  <si>
-    <t>0.2073091067797041</t>
-  </si>
-  <si>
-    <t>0.26940873845741536</t>
-  </si>
-  <si>
-    <t>0.26442923223338793</t>
-  </si>
-  <si>
-    <t>0.1724219462387864</t>
-  </si>
-  <si>
-    <t>0.13717122983238922</t>
-  </si>
-  <si>
-    <t>0.1983056960838603</t>
-  </si>
-  <si>
-    <t>0.1697162594151356</t>
-  </si>
-  <si>
-    <t>0.16927933387580896</t>
-  </si>
-  <si>
-    <t>0.1390951894684303</t>
-  </si>
-  <si>
-    <t>0.12005170052759659</t>
-  </si>
-  <si>
-    <t>0.1271555201832902</t>
-  </si>
-  <si>
-    <t>0.3112173739565132</t>
-  </si>
-  <si>
-    <t>0.2476809525466632</t>
-  </si>
-  <si>
-    <t>0.20788055089904578</t>
-  </si>
-  <si>
-    <t>0.17660693795598226</t>
-  </si>
-  <si>
-    <t>0.17600356718478002</t>
-  </si>
-  <si>
-    <t>0.181902742521992</t>
+    <t>last</t>
   </si>
 </sst>
 </file>
@@ -274,254 +108,392 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.3803149606299209E-2"/>
-          <c:y val="0.40907407407407409"/>
-          <c:w val="0.90286351706036749"/>
-          <c:h val="0.38660542432195977"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>distance</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$E:$E</c:f>
+              <c:f>Blad1!$E$2:$E$150</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1048576"/>
+                <c:ptCount val="149"/>
+                <c:pt idx="0">
+                  <c:v>0.25822784827393602</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.11612819053479199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.130365330179504</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.28937574172306502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.13633115512315699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.247946803031761</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.20879652971548701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.347756163074247</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.28090789204468303</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.179693324035336</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.180398410363968</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.224325479344571</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.27544266805608097</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.32596346610592503</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.131017805334044</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.199613515283589</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.22473430028538599</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.24720502825846999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.182423518200624</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>9.0653099624394703E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>0.30939332343863901</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>0.191376764361576</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>0.181976283852708</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>0.117228049977608</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>0.25595416131677101</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>0.15489158293399299</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>7.8822192000834901E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>0.22032454339747901</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>0.23479460176716199</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>0.181176277916683</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.28813386216791897</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.29868191552286</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>0.14550500436669001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>0.349540214400335</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>0.11702270756949799</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>0.20304268102421899</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>0.207358606398201</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>0.24269776523380701</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>0.130054891469391</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>0.29211588888628498</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>0.20730910677970399</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>0.26940873845741498</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>0.26442923223338699</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>0.17242194623878601</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>0.137171229832389</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>0.19830569608386001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>0.16971625941513499</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>0.16927933387580801</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>0.13909518946843</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>0.12005170052759601</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>0.12715552018328999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0</c:v>
+                  <c:v>0.311217373956513</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>0.247680952546663</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>0.207880550899045</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0</c:v>
+                  <c:v>0.17660693795598201</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0</c:v>
+                  <c:v>0.17600356718478</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
+                  <c:v>0.18190274252199201</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.14965271651265799</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.214589110079169</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.25195418148672999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.5787293844189396E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.16905889605643801</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.216930701097031</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.215908343896278</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.25077806265088398</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.32926556235378501</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.248586778283128</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.28506249962532199</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.151563290742706</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.19666314440539201</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.21789428598045299</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.24466486257509101</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.29782283953001099</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.14052856946800599</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.21468610097365101</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.22645322630627401</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.24846450732874301</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.22839335384696899</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.181470458576938</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.8591764023511793E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.22558367950396599</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.13551759816607001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.21600084348300699</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.21538445303137899</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.19595125949571199</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.254014014377835</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.197435881681816</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.197084399890394</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.245799587500447</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.28916566152311102</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.23279071979608801</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.37690722880091398</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.33336962196938602</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.18622109956819299</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.23105886558598199</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.141752632933735</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.14278934654966199</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.105733262014173</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.238721742247166</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.360257749852749</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.12956343012759799</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.13391210694042199</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.28626388635722999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.15664910872601701</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.21179021658012601</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.257854607963168</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.191857135551396</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.263173503916035</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.29785372743321198</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.20685811008243801</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.14494246005818201</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.205440047956296</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.13714639990493299</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.284106405547079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-11A8-4087-85C0-DA2F02AF5F66}"/>
+              <c16:uniqueId val="{00000000-5536-4249-A973-378924F74EBA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -533,12 +505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="421955152"/>
-        <c:axId val="421952656"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="421955152"/>
+        <c:axId val="757386351"/>
+        <c:axId val="757388431"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="757386351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,15 +551,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421952656"/>
+        <c:crossAx val="757388431"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="421952656"/>
+        <c:axId val="757388431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,9 +607,9 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421955152"/>
+        <c:crossAx val="757386351"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1255,23 +1223,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Grafiek 3">
+        <xdr:cNvPr id="2" name="Grafiek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3797A777-B2A5-4061-B322-A569C07EC7F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B7712E-FB74-4C7E-BB3A-B65AAFB8DBF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1589,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE9E3DD-9980-4393-B1DA-B21B43407FBB}">
-  <dimension ref="D2:E58"/>
+  <dimension ref="D2:V156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1600,460 +1568,1604 @@
     <col min="5" max="5" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>0.25822784827393602</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0.11612819053479199</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0.130365330179504</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0.28937574172306502</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0.13633115512315699</v>
+      </c>
+      <c r="F6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0.247946803031761</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0.20879652971548701</v>
+      </c>
+      <c r="F8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0.347756163074247</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0.28090789204468303</v>
+      </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0.179693324035336</v>
+      </c>
+      <c r="F11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>0.180398410363968</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>0.224325479344571</v>
+      </c>
+      <c r="F13">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>0.27544266805608097</v>
+      </c>
+      <c r="F14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>0.32596346610592503</v>
+      </c>
+      <c r="F15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>0.131017805334044</v>
+      </c>
+      <c r="F16">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>0.199613515283589</v>
+      </c>
+      <c r="F17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>17</v>
       </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>0.22473430028538599</v>
+      </c>
+      <c r="F18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19">
         <v>18</v>
       </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>0.24720502825846999</v>
+      </c>
+      <c r="F19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>0.182423518200624</v>
+      </c>
+      <c r="F20">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21">
         <v>20</v>
       </c>
-      <c r="E21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>9.0653099624394703E-2</v>
+      </c>
+      <c r="F21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>0.30939332343863901</v>
+      </c>
+      <c r="F22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23">
         <v>22</v>
       </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>0.191376764361576</v>
+      </c>
+      <c r="F23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D24">
         <v>23</v>
       </c>
-      <c r="E24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>0.181976283852708</v>
+      </c>
+      <c r="F24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>24</v>
       </c>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>0.117228049977608</v>
+      </c>
+      <c r="F25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D26">
         <v>25</v>
       </c>
-      <c r="E26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>0.25595416131677101</v>
+      </c>
+      <c r="F26">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D27">
         <v>26</v>
       </c>
-      <c r="E27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>0.15489158293399299</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D28">
         <v>27</v>
       </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>7.8822192000834901E-2</v>
+      </c>
+      <c r="F28">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D29">
         <v>28</v>
       </c>
-      <c r="E29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>0.22032454339747901</v>
+      </c>
+      <c r="F29">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D30">
         <v>29</v>
       </c>
-      <c r="E30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>0.23479460176716199</v>
+      </c>
+      <c r="F30">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D31">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>0.181176277916683</v>
+      </c>
+      <c r="F31">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D32">
         <v>31</v>
       </c>
-      <c r="E32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>0.28813386216791897</v>
+      </c>
+      <c r="F32">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D33">
         <v>32</v>
       </c>
-      <c r="E33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>0.29868191552286</v>
+      </c>
+      <c r="F33">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D34">
         <v>33</v>
       </c>
-      <c r="E34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>0.14550500436669001</v>
+      </c>
+      <c r="F34">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D35">
         <v>34</v>
       </c>
-      <c r="E35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>0.349540214400335</v>
+      </c>
+      <c r="F35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D36">
         <v>35</v>
       </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>0.11702270756949799</v>
+      </c>
+      <c r="F36">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D37">
         <v>36</v>
       </c>
-      <c r="E37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>0.20304268102421899</v>
+      </c>
+      <c r="F37">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D38">
         <v>37</v>
       </c>
-      <c r="E38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>0.207358606398201</v>
+      </c>
+      <c r="F38">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D39">
         <v>38</v>
       </c>
-      <c r="E39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>0.24269776523380701</v>
+      </c>
+      <c r="F39">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D40">
         <v>39</v>
       </c>
-      <c r="E40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>0.130054891469391</v>
+      </c>
+      <c r="F40">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D41">
         <v>40</v>
       </c>
-      <c r="E41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>0.29211588888628498</v>
+      </c>
+      <c r="F41">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D42">
         <v>41</v>
       </c>
-      <c r="E42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>0.20730910677970399</v>
+      </c>
+      <c r="F42">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D43">
         <v>42</v>
       </c>
-      <c r="E43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>0.26940873845741498</v>
+      </c>
+      <c r="F43">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D44">
         <v>43</v>
       </c>
-      <c r="E44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>0.26442923223338699</v>
+      </c>
+      <c r="F44">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D45">
         <v>44</v>
       </c>
-      <c r="E45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>0.17242194623878601</v>
+      </c>
+      <c r="F45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D46">
         <v>45</v>
       </c>
-      <c r="E46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>0.137171229832389</v>
+      </c>
+      <c r="F46">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D47">
         <v>46</v>
       </c>
-      <c r="E47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>0.19830569608386001</v>
+      </c>
+      <c r="F47">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D48">
         <v>47</v>
       </c>
-      <c r="E48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>0.16971625941513499</v>
+      </c>
+      <c r="F48">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D49">
         <v>48</v>
       </c>
-      <c r="E49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>0.16927933387580801</v>
+      </c>
+      <c r="F49">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D50">
         <v>49</v>
       </c>
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>0.13909518946843</v>
+      </c>
+      <c r="F50">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D51">
         <v>50</v>
       </c>
-      <c r="E51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>0.12005170052759601</v>
+      </c>
+      <c r="F51">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D52">
         <v>51</v>
       </c>
-      <c r="E52" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>0.12715552018328999</v>
+      </c>
+      <c r="F52">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D53">
         <v>52</v>
       </c>
-      <c r="E53" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>0.311217373956513</v>
+      </c>
+      <c r="F53">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D54">
         <v>53</v>
       </c>
-      <c r="E54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>0.247680952546663</v>
+      </c>
+      <c r="F54">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D55">
         <v>54</v>
       </c>
-      <c r="E55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>0.207880550899045</v>
+      </c>
+      <c r="F55">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D56">
         <v>55</v>
       </c>
-      <c r="E56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>0.17660693795598201</v>
+      </c>
+      <c r="F56">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D57">
         <v>56</v>
       </c>
-      <c r="E57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>0.17600356718478</v>
+      </c>
+      <c r="F57">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D58">
         <v>57</v>
       </c>
-      <c r="E58" t="s">
-        <v>56</v>
+      <c r="E58">
+        <v>0.18190274252199201</v>
+      </c>
+      <c r="F58">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>58</v>
+      </c>
+      <c r="F59">
+        <v>228</v>
+      </c>
+      <c r="G59" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>58</v>
+      </c>
+      <c r="I59">
+        <v>0.131017805334044</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>59</v>
+      </c>
+      <c r="E60">
+        <v>0.14965271651265799</v>
+      </c>
+      <c r="F60">
+        <v>232</v>
+      </c>
+      <c r="H60">
+        <v>59</v>
+      </c>
+      <c r="I60">
+        <v>0.199613515283589</v>
+      </c>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>60</v>
+      </c>
+      <c r="E61">
+        <v>0.214589110079169</v>
+      </c>
+      <c r="F61">
+        <v>236</v>
+      </c>
+      <c r="H61">
+        <v>60</v>
+      </c>
+      <c r="I61">
+        <v>0.22473430028538599</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>61</v>
+      </c>
+      <c r="E62">
+        <v>0.25195418148672999</v>
+      </c>
+      <c r="F62">
+        <v>240</v>
+      </c>
+      <c r="H62">
+        <v>61</v>
+      </c>
+      <c r="I62">
+        <v>0.24720502825846999</v>
+      </c>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>62</v>
+      </c>
+      <c r="E63">
+        <v>6.5787293844189396E-2</v>
+      </c>
+      <c r="F63">
+        <v>244</v>
+      </c>
+      <c r="H63">
+        <v>62</v>
+      </c>
+      <c r="I63">
+        <v>0.182423518200624</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>63</v>
+      </c>
+      <c r="E64">
+        <v>0.16905889605643801</v>
+      </c>
+      <c r="F64">
+        <v>248</v>
+      </c>
+      <c r="H64">
+        <v>63</v>
+      </c>
+      <c r="I64">
+        <v>9.0653099624394703E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>64</v>
+      </c>
+      <c r="E65">
+        <v>0.216930701097031</v>
+      </c>
+      <c r="F65">
+        <v>252</v>
+      </c>
+      <c r="H65">
+        <v>64</v>
+      </c>
+      <c r="I65">
+        <v>0.30939332343863901</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>65</v>
+      </c>
+      <c r="E66">
+        <v>0.215908343896278</v>
+      </c>
+      <c r="F66">
+        <v>256</v>
+      </c>
+      <c r="H66">
+        <v>65</v>
+      </c>
+      <c r="I66">
+        <v>0.191376764361576</v>
+      </c>
+    </row>
+    <row r="67" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>66</v>
+      </c>
+      <c r="E67">
+        <v>0.25077806265088398</v>
+      </c>
+      <c r="F67">
+        <v>260</v>
+      </c>
+      <c r="H67">
+        <v>66</v>
+      </c>
+      <c r="I67">
+        <v>0.181976283852708</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>67</v>
+      </c>
+      <c r="E68">
+        <v>0.32926556235378501</v>
+      </c>
+      <c r="F68">
+        <v>264</v>
+      </c>
+      <c r="H68">
+        <v>67</v>
+      </c>
+      <c r="I68">
+        <v>0.117228049977608</v>
+      </c>
+    </row>
+    <row r="69" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>68</v>
+      </c>
+      <c r="E69">
+        <v>0.248586778283128</v>
+      </c>
+      <c r="F69">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>69</v>
+      </c>
+      <c r="E70">
+        <v>0.28506249962532199</v>
+      </c>
+      <c r="F70">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>70</v>
+      </c>
+      <c r="E71">
+        <v>0.151563290742706</v>
+      </c>
+      <c r="F71">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>71</v>
+      </c>
+      <c r="E72">
+        <v>0.19666314440539201</v>
+      </c>
+      <c r="F72">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>72</v>
+      </c>
+      <c r="E73">
+        <v>0.21789428598045299</v>
+      </c>
+      <c r="F73">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="74" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>73</v>
+      </c>
+      <c r="E74">
+        <v>0.24466486257509101</v>
+      </c>
+      <c r="F74">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>74</v>
+      </c>
+      <c r="E75">
+        <v>0.29782283953001099</v>
+      </c>
+      <c r="F75">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="76" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>75</v>
+      </c>
+      <c r="E76">
+        <v>0.14052856946800599</v>
+      </c>
+      <c r="F76">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="77" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>76</v>
+      </c>
+      <c r="E77">
+        <v>0.21468610097365101</v>
+      </c>
+      <c r="F77">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>77</v>
+      </c>
+      <c r="E78">
+        <v>0.22645322630627401</v>
+      </c>
+      <c r="F78">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="79" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>78</v>
+      </c>
+      <c r="E79">
+        <v>0.24846450732874301</v>
+      </c>
+      <c r="F79">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="80" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>79</v>
+      </c>
+      <c r="E80">
+        <v>0.22839335384696899</v>
+      </c>
+      <c r="F80">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>80</v>
+      </c>
+      <c r="E81">
+        <v>0.181470458576938</v>
+      </c>
+      <c r="F81">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>81</v>
+      </c>
+      <c r="E82">
+        <v>8.8591764023511793E-2</v>
+      </c>
+      <c r="F82">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>82</v>
+      </c>
+      <c r="E83">
+        <v>0.22558367950396599</v>
+      </c>
+      <c r="F83">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>83</v>
+      </c>
+      <c r="E84">
+        <v>0.13551759816607001</v>
+      </c>
+      <c r="F84">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>84</v>
+      </c>
+      <c r="E85">
+        <v>0.21600084348300699</v>
+      </c>
+      <c r="F85">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>85</v>
+      </c>
+      <c r="E86">
+        <v>0.21538445303137899</v>
+      </c>
+      <c r="F86">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>86</v>
+      </c>
+      <c r="E87">
+        <v>0.19595125949571199</v>
+      </c>
+      <c r="F87">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>87</v>
+      </c>
+      <c r="E88">
+        <v>0.254014014377835</v>
+      </c>
+      <c r="F88">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>88</v>
+      </c>
+      <c r="E89">
+        <v>0.197435881681816</v>
+      </c>
+      <c r="F89">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>89</v>
+      </c>
+      <c r="E90">
+        <v>0.197084399890394</v>
+      </c>
+      <c r="F90">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>90</v>
+      </c>
+      <c r="E91">
+        <v>0.245799587500447</v>
+      </c>
+      <c r="F91">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>91</v>
+      </c>
+      <c r="E92">
+        <v>0.28916566152311102</v>
+      </c>
+      <c r="F92">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>92</v>
+      </c>
+      <c r="E93">
+        <v>0.23279071979608801</v>
+      </c>
+      <c r="F93">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>93</v>
+      </c>
+      <c r="E94">
+        <v>0.37690722880091398</v>
+      </c>
+      <c r="F94">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>94</v>
+      </c>
+      <c r="E95">
+        <v>0.33336962196938602</v>
+      </c>
+      <c r="F95">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>95</v>
+      </c>
+      <c r="E96">
+        <v>0.18622109956819299</v>
+      </c>
+      <c r="F96">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>96</v>
+      </c>
+      <c r="E97">
+        <v>0.23105886558598199</v>
+      </c>
+      <c r="F97">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>97</v>
+      </c>
+      <c r="E98">
+        <v>0.141752632933735</v>
+      </c>
+      <c r="F98">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>98</v>
+      </c>
+      <c r="E99">
+        <v>0.14278934654966199</v>
+      </c>
+      <c r="F99">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>99</v>
+      </c>
+      <c r="E100">
+        <v>0.105733262014173</v>
+      </c>
+      <c r="F100">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>100</v>
+      </c>
+      <c r="E101">
+        <v>0.238721742247166</v>
+      </c>
+      <c r="F101">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>101</v>
+      </c>
+      <c r="E102">
+        <v>0.360257749852749</v>
+      </c>
+      <c r="F102">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>102</v>
+      </c>
+      <c r="E103">
+        <v>0.12956343012759799</v>
+      </c>
+      <c r="F103">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>103</v>
+      </c>
+      <c r="E104">
+        <v>0.13391210694042199</v>
+      </c>
+      <c r="F104">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>104</v>
+      </c>
+      <c r="E105">
+        <v>0.28626388635722999</v>
+      </c>
+      <c r="F105">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>105</v>
+      </c>
+      <c r="E106">
+        <v>0.15664910872601701</v>
+      </c>
+      <c r="F106">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>106</v>
+      </c>
+      <c r="E107">
+        <v>0.21179021658012601</v>
+      </c>
+      <c r="F107">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>107</v>
+      </c>
+      <c r="E108">
+        <v>0.257854607963168</v>
+      </c>
+      <c r="F108">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>108</v>
+      </c>
+      <c r="E109">
+        <v>0.191857135551396</v>
+      </c>
+      <c r="F109">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>109</v>
+      </c>
+      <c r="E110">
+        <v>0.263173503916035</v>
+      </c>
+      <c r="F110">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>110</v>
+      </c>
+      <c r="E111">
+        <v>0.29785372743321198</v>
+      </c>
+      <c r="F111">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>111</v>
+      </c>
+      <c r="E112">
+        <v>0.20685811008243801</v>
+      </c>
+      <c r="F112">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="113" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>112</v>
+      </c>
+      <c r="E113">
+        <v>0.14494246005818201</v>
+      </c>
+      <c r="F113">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="114" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>113</v>
+      </c>
+      <c r="E114">
+        <v>0.205440047956296</v>
+      </c>
+      <c r="F114">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="115" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>114</v>
+      </c>
+      <c r="E115">
+        <v>0.13714639990493299</v>
+      </c>
+      <c r="F115">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="116" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>115</v>
+      </c>
+      <c r="E116">
+        <v>0.284106405547079</v>
+      </c>
+      <c r="F116">
+        <v>456</v>
+      </c>
+      <c r="G116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>116</v>
+      </c>
+      <c r="F117">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="124" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="U124">
+        <v>68</v>
+      </c>
+      <c r="V124">
+        <v>0.25595416131677101</v>
+      </c>
+    </row>
+    <row r="125" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="U125">
+        <v>69</v>
+      </c>
+      <c r="V125">
+        <v>0.15489158293399299</v>
+      </c>
+    </row>
+    <row r="126" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="U126">
+        <v>70</v>
+      </c>
+      <c r="V126">
+        <v>7.8822192000834901E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="U127">
+        <v>71</v>
+      </c>
+      <c r="V127">
+        <v>0.22032454339747901</v>
+      </c>
+    </row>
+    <row r="128" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="U128">
+        <v>72</v>
+      </c>
+      <c r="V128">
+        <v>0.23479460176716199</v>
+      </c>
+    </row>
+    <row r="129" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U129">
+        <v>73</v>
+      </c>
+      <c r="V129">
+        <v>0.181176277916683</v>
+      </c>
+    </row>
+    <row r="130" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U130">
+        <v>74</v>
+      </c>
+      <c r="V130">
+        <v>0.28813386216791897</v>
+      </c>
+    </row>
+    <row r="131" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U131">
+        <v>75</v>
+      </c>
+      <c r="V131">
+        <v>0.29868191552286</v>
+      </c>
+    </row>
+    <row r="132" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U132">
+        <v>76</v>
+      </c>
+      <c r="V132">
+        <v>0.14550500436669001</v>
+      </c>
+    </row>
+    <row r="133" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U133">
+        <v>77</v>
+      </c>
+      <c r="V133">
+        <v>0.349540214400335</v>
+      </c>
+    </row>
+    <row r="134" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U134">
+        <v>78</v>
+      </c>
+      <c r="V134">
+        <v>0.11702270756949799</v>
+      </c>
+    </row>
+    <row r="135" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U135">
+        <v>79</v>
+      </c>
+      <c r="V135">
+        <v>0.20304268102421899</v>
+      </c>
+    </row>
+    <row r="136" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U136">
+        <v>80</v>
+      </c>
+      <c r="V136">
+        <v>0.207358606398201</v>
+      </c>
+    </row>
+    <row r="137" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U137">
+        <v>81</v>
+      </c>
+      <c r="V137">
+        <v>0.24269776523380701</v>
+      </c>
+    </row>
+    <row r="138" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U138">
+        <v>82</v>
+      </c>
+      <c r="V138">
+        <v>0.130054891469391</v>
+      </c>
+    </row>
+    <row r="139" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U139">
+        <v>83</v>
+      </c>
+      <c r="V139">
+        <v>0.29211588888628498</v>
+      </c>
+    </row>
+    <row r="140" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U140">
+        <v>84</v>
+      </c>
+      <c r="V140">
+        <v>0.20730910677970399</v>
+      </c>
+    </row>
+    <row r="141" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U141">
+        <v>85</v>
+      </c>
+      <c r="V141">
+        <v>0.26940873845741498</v>
+      </c>
+    </row>
+    <row r="142" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U142">
+        <v>86</v>
+      </c>
+      <c r="V142">
+        <v>0.26442923223338699</v>
+      </c>
+    </row>
+    <row r="143" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U143">
+        <v>87</v>
+      </c>
+      <c r="V143">
+        <v>0.17242194623878601</v>
+      </c>
+    </row>
+    <row r="144" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U144">
+        <v>88</v>
+      </c>
+      <c r="V144">
+        <v>0.137171229832389</v>
+      </c>
+    </row>
+    <row r="145" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U145">
+        <v>89</v>
+      </c>
+      <c r="V145">
+        <v>0.19830569608386001</v>
+      </c>
+    </row>
+    <row r="146" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U146">
+        <v>90</v>
+      </c>
+      <c r="V146">
+        <v>0.16971625941513499</v>
+      </c>
+    </row>
+    <row r="147" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U147">
+        <v>91</v>
+      </c>
+      <c r="V147">
+        <v>0.16927933387580801</v>
+      </c>
+    </row>
+    <row r="148" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U148">
+        <v>92</v>
+      </c>
+      <c r="V148">
+        <v>0.13909518946843</v>
+      </c>
+    </row>
+    <row r="149" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U149">
+        <v>93</v>
+      </c>
+      <c r="V149">
+        <v>0.12005170052759601</v>
+      </c>
+    </row>
+    <row r="150" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U150">
+        <v>94</v>
+      </c>
+      <c r="V150">
+        <v>0.12715552018328999</v>
+      </c>
+    </row>
+    <row r="151" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U151">
+        <v>95</v>
+      </c>
+      <c r="V151">
+        <v>0.311217373956513</v>
+      </c>
+    </row>
+    <row r="152" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U152">
+        <v>96</v>
+      </c>
+      <c r="V152">
+        <v>0.247680952546663</v>
+      </c>
+    </row>
+    <row r="153" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U153">
+        <v>97</v>
+      </c>
+      <c r="V153">
+        <v>0.207880550899045</v>
+      </c>
+    </row>
+    <row r="154" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U154">
+        <v>98</v>
+      </c>
+      <c r="V154">
+        <v>0.17660693795598201</v>
+      </c>
+    </row>
+    <row r="155" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U155">
+        <v>99</v>
+      </c>
+      <c r="V155">
+        <v>0.17600356718478</v>
+      </c>
+    </row>
+    <row r="156" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U156">
+        <v>100</v>
+      </c>
+      <c r="V156">
+        <v>0.18190274252199201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make distribution from face rec data
</commit_message>
<xml_diff>
--- a/data/before_recognition.xlsx
+++ b/data/before_recognition.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murie\Documents\school\master\1B\Introduction2Biometrics\project_git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD754C8-26EC-4D08-B94C-243A799D2429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B923F3-0351-467B-AAA3-318043FFABD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD5D7408-1DBF-4EC5-8EFD-A3374FDE4ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Blad1!$F$2:$F$115</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Blad1!$D$2:$D$150</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$E$2:$E$116</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$F$2:$F$150</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$G$2:$G$150</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$F$2:$F$115</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2170,7 +2178,195 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.4</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{E7F6931C-95A1-45E9-BFE5-E3BA7212FB60}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Distance2self</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{00000001-681F-493E-9B17-3846CA7DA94E}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>distance2otherNoExp</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{00000002-681F-493E-9B17-3846CA7DA94E}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Distance2otherExp</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.00999999978"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{A23F4032-7F71-44D8-B9FC-78BDF8F2589F}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2726,6 +2922,1022 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2762,6 +3974,162 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Grafiek 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0678CDA7-0DD2-47E5-8F53-BB7EE9CB15A1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7406640" y="3044190"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="nl-NL" sz="1100"/>
+                <a:t>Deze grafiek is niet beschikbaar in uw versie van Excel.
+Als u deze vorm bewerkt of deze werkmap opslaat in een andere bestandsindeling, wordt de grafiek onherstelbaar beschadigd.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Grafiek 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD90DE25-A568-45EB-802B-5E754271A31C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7383780" y="5863590"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="nl-NL" sz="1100"/>
+                <a:t>Deze grafiek is niet beschikbaar in uw versie van Excel.
+Als u deze vorm bewerkt of deze werkmap opslaat in een andere bestandsindeling, wordt de grafiek onherstelbaar beschadigd.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3067,7 +4435,7 @@
   <dimension ref="C1:I116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="D1" sqref="D1:G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>